<commit_message>
chore: update reference Excel file
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/+qPCR_진정_20260205_1424.xlsx
+++ b/+qPCR_진정_20260205_1424.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\minsangkim\qPCR-data-analysis-platform-v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3C467D-04E4-4F7E-94E6-C6EAEC841F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1120FD-B677-41D5-AE55-2BB0770AF902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3300" yWindow="2085" windowWidth="30315" windowHeight="13950" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11196" yWindow="1020" windowWidth="19956" windowHeight="10872" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis_Parameters" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,12 @@
     <sheet name="Summary" sheetId="6" r:id="rId6"/>
     <sheet name="ADD THIS" sheetId="7" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="178">
   <si>
     <t>Date</t>
   </si>
@@ -915,7 +912,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'ADD THIS'!$E$3:$E$19</c:f>
+                <c:f>'ADD THIS'!$E$6:$E$22</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
@@ -975,7 +972,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'ADD THIS'!$E$3:$E$19</c:f>
+                <c:f>'ADD THIS'!$E$6:$E$22</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
@@ -1049,7 +1046,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'ADD THIS'!$C$3:$C$19</c:f>
+              <c:f>'ADD THIS'!$C$6:$C$22</c:f>
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
@@ -1108,7 +1105,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ADD THIS'!$D$3:$D$19</c:f>
+              <c:f>'ADD THIS'!$D$6:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -2019,16 +2016,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>13607</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>553936</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152153</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>639536</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>40821</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>514846</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>179366</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2056,68 +2053,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="77">
-          <cell r="P77">
-            <v>4.4744223060774739E-2</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="P78">
-            <v>5.9252874261945733E-2</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="P79">
-            <v>4.5783867831113434E-2</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="P80">
-            <v>0.10771791881063336</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="P81">
-            <v>0.13954479079570678</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="P82">
-            <v>7.350307940811393E-2</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="P83">
-            <v>0.16574074369078051</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="P84">
-            <v>2.1791147951429089E-2</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="P85">
-            <v>3.4858009364500037E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2413,9 +2348,9 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2441,7 +2376,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2479,9 +2414,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2498,7 +2433,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2512,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2526,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2540,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2554,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2568,7 +2503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2582,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2596,7 +2531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2610,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2624,7 +2559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2638,7 +2573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2652,7 +2587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2666,7 +2601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2680,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2694,7 +2629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2708,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2722,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2736,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2750,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2764,7 +2699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2790,9 +2725,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -2812,7 +2747,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2832,7 +2767,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2852,7 +2787,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2872,7 +2807,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -2892,7 +2827,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -2912,7 +2847,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -2932,7 +2867,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -2952,7 +2887,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -2972,7 +2907,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2992,7 +2927,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -3012,7 +2947,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -3032,7 +2967,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -3052,7 +2987,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -3072,7 +3007,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -3092,7 +3027,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -3112,7 +3047,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -3132,7 +3067,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3152,7 +3087,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3172,7 +3107,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -3192,7 +3127,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -3212,7 +3147,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -3232,7 +3167,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -3252,7 +3187,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -3272,7 +3207,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -3292,7 +3227,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -3312,7 +3247,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -3332,7 +3267,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -3352,7 +3287,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -3372,7 +3307,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -3392,7 +3327,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -3412,7 +3347,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -3432,7 +3367,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -3452,7 +3387,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -3472,7 +3407,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -3492,7 +3427,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -3512,7 +3447,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -3532,7 +3467,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -3552,7 +3487,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -3572,7 +3507,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -3592,7 +3527,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -3612,7 +3547,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -3632,7 +3567,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -3652,7 +3587,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -3672,7 +3607,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -3692,7 +3627,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -3712,7 +3647,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -3732,7 +3667,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -3752,7 +3687,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -3772,7 +3707,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -3792,7 +3727,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -3812,7 +3747,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>95</v>
       </c>
@@ -3832,7 +3767,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>96</v>
       </c>
@@ -3852,7 +3787,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>97</v>
       </c>
@@ -3872,7 +3807,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -3892,7 +3827,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>99</v>
       </c>
@@ -3912,7 +3847,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -3932,7 +3867,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>101</v>
       </c>
@@ -3952,7 +3887,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>102</v>
       </c>
@@ -3972,7 +3907,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>103</v>
       </c>
@@ -3992,7 +3927,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>104</v>
       </c>
@@ -4012,7 +3947,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>105</v>
       </c>
@@ -4032,7 +3967,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>106</v>
       </c>
@@ -4052,7 +3987,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>107</v>
       </c>
@@ -4072,7 +4007,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>108</v>
       </c>
@@ -4092,7 +4027,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>109</v>
       </c>
@@ -4112,7 +4047,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>110</v>
       </c>
@@ -4132,7 +4067,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>111</v>
       </c>
@@ -4152,7 +4087,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>112</v>
       </c>
@@ -4172,7 +4107,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>113</v>
       </c>
@@ -4192,7 +4127,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>114</v>
       </c>
@@ -4212,7 +4147,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>115</v>
       </c>
@@ -4232,7 +4167,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>116</v>
       </c>
@@ -4252,7 +4187,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>117</v>
       </c>
@@ -4272,7 +4207,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>118</v>
       </c>
@@ -4292,7 +4227,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>119</v>
       </c>
@@ -4312,7 +4247,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>120</v>
       </c>
@@ -4332,7 +4267,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>121</v>
       </c>
@@ -4352,7 +4287,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>122</v>
       </c>
@@ -4372,7 +4307,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>123</v>
       </c>
@@ -4392,7 +4327,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>124</v>
       </c>
@@ -4412,7 +4347,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>125</v>
       </c>
@@ -4432,7 +4367,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>126</v>
       </c>
@@ -4452,7 +4387,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>127</v>
       </c>
@@ -4472,7 +4407,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>128</v>
       </c>
@@ -4492,7 +4427,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>129</v>
       </c>
@@ -4512,7 +4447,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>130</v>
       </c>
@@ -4532,7 +4467,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>131</v>
       </c>
@@ -4552,7 +4487,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>132</v>
       </c>
@@ -4572,7 +4507,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>133</v>
       </c>
@@ -4592,7 +4527,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>134</v>
       </c>
@@ -4612,7 +4547,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>135</v>
       </c>
@@ -4632,7 +4567,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>136</v>
       </c>
@@ -4652,7 +4587,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>137</v>
       </c>
@@ -4672,7 +4607,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>138</v>
       </c>
@@ -4692,7 +4627,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>139</v>
       </c>
@@ -4712,7 +4647,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>140</v>
       </c>
@@ -4732,7 +4667,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>45</v>
       </c>
@@ -4752,7 +4687,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>46</v>
       </c>
@@ -4772,7 +4707,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -4792,7 +4727,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -4812,7 +4747,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>49</v>
       </c>
@@ -4832,7 +4767,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>50</v>
       </c>
@@ -4852,7 +4787,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>51</v>
       </c>
@@ -4872,7 +4807,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>52</v>
       </c>
@@ -4892,7 +4827,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>53</v>
       </c>
@@ -4912,7 +4847,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>54</v>
       </c>
@@ -4932,7 +4867,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
         <v>55</v>
       </c>
@@ -4952,7 +4887,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
         <v>56</v>
       </c>
@@ -4972,7 +4907,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>57</v>
       </c>
@@ -4992,7 +4927,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>58</v>
       </c>
@@ -5012,7 +4947,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
         <v>59</v>
       </c>
@@ -5032,7 +4967,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
         <v>60</v>
       </c>
@@ -5052,7 +4987,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
         <v>61</v>
       </c>
@@ -5072,7 +5007,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
         <v>62</v>
       </c>
@@ -5092,7 +5027,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
         <v>63</v>
       </c>
@@ -5112,7 +5047,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
         <v>64</v>
       </c>
@@ -5132,7 +5067,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
         <v>65</v>
       </c>
@@ -5152,7 +5087,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
         <v>66</v>
       </c>
@@ -5172,7 +5107,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
         <v>67</v>
       </c>
@@ -5192,7 +5127,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
         <v>68</v>
       </c>
@@ -5212,7 +5147,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
         <v>69</v>
       </c>
@@ -5232,7 +5167,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
         <v>70</v>
       </c>
@@ -5252,7 +5187,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
         <v>71</v>
       </c>
@@ -5272,7 +5207,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
         <v>72</v>
       </c>
@@ -5292,7 +5227,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
         <v>73</v>
       </c>
@@ -5312,7 +5247,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>74</v>
       </c>
@@ -5332,7 +5267,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>75</v>
       </c>
@@ -5352,7 +5287,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>76</v>
       </c>
@@ -5372,7 +5307,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>77</v>
       </c>
@@ -5392,7 +5327,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>78</v>
       </c>
@@ -5412,7 +5347,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
         <v>79</v>
       </c>
@@ -5432,7 +5367,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
         <v>80</v>
       </c>
@@ -5452,7 +5387,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
         <v>81</v>
       </c>
@@ -5472,7 +5407,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
         <v>82</v>
       </c>
@@ -5492,7 +5427,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
         <v>83</v>
       </c>
@@ -5512,7 +5447,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
         <v>84</v>
       </c>
@@ -5532,7 +5467,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
         <v>85</v>
       </c>
@@ -5552,7 +5487,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
         <v>86</v>
       </c>
@@ -5572,7 +5507,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
         <v>87</v>
       </c>
@@ -5592,7 +5527,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
         <v>88</v>
       </c>
@@ -5612,7 +5547,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
         <v>89</v>
       </c>
@@ -5632,7 +5567,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
         <v>90</v>
       </c>
@@ -5652,7 +5587,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
         <v>91</v>
       </c>
@@ -5672,7 +5607,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
         <v>92</v>
       </c>
@@ -5692,7 +5627,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
         <v>93</v>
       </c>
@@ -5712,7 +5647,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
         <v>94</v>
       </c>
@@ -5732,7 +5667,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
         <v>95</v>
       </c>
@@ -5752,7 +5687,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
         <v>96</v>
       </c>
@@ -5772,7 +5707,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
         <v>97</v>
       </c>
@@ -5792,7 +5727,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
         <v>98</v>
       </c>
@@ -5812,7 +5747,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
         <v>99</v>
       </c>
@@ -5832,7 +5767,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
         <v>100</v>
       </c>
@@ -5852,7 +5787,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
         <v>101</v>
       </c>
@@ -5872,7 +5807,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
         <v>102</v>
       </c>
@@ -5892,7 +5827,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
         <v>103</v>
       </c>
@@ -5912,7 +5847,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
         <v>104</v>
       </c>
@@ -5932,7 +5867,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
         <v>105</v>
       </c>
@@ -5952,7 +5887,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
         <v>106</v>
       </c>
@@ -5972,7 +5907,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
         <v>107</v>
       </c>
@@ -5992,7 +5927,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
         <v>108</v>
       </c>
@@ -6012,7 +5947,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
         <v>109</v>
       </c>
@@ -6032,7 +5967,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
         <v>110</v>
       </c>
@@ -6052,7 +5987,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
         <v>111</v>
       </c>
@@ -6072,7 +6007,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A165" t="s">
         <v>112</v>
       </c>
@@ -6092,7 +6027,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
         <v>113</v>
       </c>
@@ -6112,7 +6047,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A167" t="s">
         <v>114</v>
       </c>
@@ -6132,7 +6067,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A168" t="s">
         <v>115</v>
       </c>
@@ -6152,7 +6087,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A169" t="s">
         <v>116</v>
       </c>
@@ -6172,7 +6107,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A170" t="s">
         <v>117</v>
       </c>
@@ -6192,7 +6127,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A171" t="s">
         <v>118</v>
       </c>
@@ -6212,7 +6147,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A172" t="s">
         <v>119</v>
       </c>
@@ -6232,7 +6167,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A173" t="s">
         <v>120</v>
       </c>
@@ -6252,7 +6187,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A174" t="s">
         <v>121</v>
       </c>
@@ -6272,7 +6207,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A175" t="s">
         <v>122</v>
       </c>
@@ -6292,7 +6227,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A176" t="s">
         <v>123</v>
       </c>
@@ -6312,7 +6247,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A177" t="s">
         <v>124</v>
       </c>
@@ -6332,7 +6267,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A178" t="s">
         <v>125</v>
       </c>
@@ -6352,7 +6287,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A179" t="s">
         <v>126</v>
       </c>
@@ -6372,7 +6307,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A180" t="s">
         <v>127</v>
       </c>
@@ -6392,7 +6327,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A181" t="s">
         <v>128</v>
       </c>
@@ -6424,9 +6359,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -6506,7 +6441,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -6574,7 +6509,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -6642,7 +6577,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -6722,7 +6657,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -6796,7 +6731,7 @@
         <v>0.32721491879155512</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -6876,7 +6811,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -6950,7 +6885,7 @@
         <v>0.17341138864868089</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -7030,7 +6965,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -7104,7 +7039,7 @@
         <v>0.33637061761339948</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -7184,7 +7119,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -7264,7 +7199,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -7344,7 +7279,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -7418,7 +7353,7 @@
         <v>0.36159153750600398</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -7498,7 +7433,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>141</v>
       </c>
@@ -7578,7 +7513,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -7658,7 +7593,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -7738,7 +7673,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -7829,12 +7764,12 @@
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AL49" sqref="S28:AL49"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -7914,7 +7849,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -7982,7 +7917,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -8050,7 +7985,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -8130,7 +8065,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -8210,7 +8145,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -8290,7 +8225,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -8364,7 +8299,7 @@
         <v>0.20576290406873399</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -8444,7 +8379,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -8524,7 +8459,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -8604,7 +8539,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -8684,7 +8619,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>142</v>
       </c>
@@ -8764,7 +8699,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>142</v>
       </c>
@@ -8844,7 +8779,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -8924,7 +8859,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -9004,7 +8939,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>142</v>
       </c>
@@ -9084,7 +9019,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>142</v>
       </c>
@@ -9164,7 +9099,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -9258,9 +9193,9 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>157</v>
@@ -9271,7 +9206,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>174</v>
@@ -9286,7 +9221,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -9294,7 +9229,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>141</v>
       </c>
@@ -9314,7 +9249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>142</v>
       </c>
@@ -9345,411 +9280,312 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297EBF2E-2F96-42D1-8277-A8F1692279B9}">
-  <dimension ref="C2:I19"/>
+  <dimension ref="C5:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E6">
         <v>4.0305316256277E-2</v>
       </c>
-      <c r="H3">
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>27.684374098719559</v>
+      </c>
+      <c r="E7">
+        <v>3.049711583205942E-2</v>
+      </c>
+      <c r="F7">
         <v>3.243230447897296E-6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4">
-        <v>27.684374098719559</v>
-      </c>
-      <c r="E4">
-        <v>3.049711583205942E-2</v>
-      </c>
-      <c r="F4">
-        <v>3.243230447897296E-6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5">
-        <v>12.820079766650441</v>
-      </c>
-      <c r="E5">
-        <v>4.7745467110812012E-2</v>
-      </c>
-      <c r="F5">
-        <v>2.3581918370932249E-5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>169</v>
-      </c>
-      <c r="H5">
-        <v>7.7404882843735637E-5</v>
-      </c>
-      <c r="I5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>30.831503375637858</v>
-      </c>
-      <c r="E6">
-        <v>2.66124448749499E-2</v>
-      </c>
-      <c r="F6">
-        <v>1.8418616256634899E-6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H6">
-        <v>3.5631412309026063E-2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7">
-        <v>23.02825732276618</v>
-      </c>
-      <c r="E7">
-        <v>1.9798989873223129E-2</v>
-      </c>
-      <c r="F7">
-        <v>5.9722024442858304E-7</v>
       </c>
       <c r="G7" t="s">
         <v>169</v>
       </c>
-      <c r="H7">
-        <v>4.7545081009094294E-3</v>
-      </c>
-      <c r="I7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D8">
-        <v>26.11849747682874</v>
+        <v>12.820079766650441</v>
       </c>
       <c r="E8">
-        <v>2.9699731885559209E-2</v>
+        <v>4.7745467110812012E-2</v>
       </c>
       <c r="F8">
-        <v>2.9766480877012392E-6</v>
+        <v>2.3581918370932249E-5</v>
       </c>
       <c r="G8" t="s">
         <v>169</v>
       </c>
-      <c r="H8">
-        <v>0.18647263181229021</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9">
-        <v>17.847704985311371</v>
+        <v>30.831503375637858</v>
       </c>
       <c r="E9">
-        <v>1.8632905978004589E-2</v>
+        <v>2.66124448749499E-2</v>
       </c>
       <c r="F9">
-        <v>4.8773719302883251E-7</v>
+        <v>1.8418616256634899E-6</v>
       </c>
       <c r="G9" t="s">
         <v>169</v>
       </c>
-      <c r="H9">
-        <v>2.2323847379642739E-4</v>
-      </c>
-      <c r="I9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10">
-        <v>16.223351676640501</v>
+        <v>23.02825732276618</v>
       </c>
       <c r="E10">
-        <v>5.022025561537951E-2</v>
+        <v>1.9798989873223129E-2</v>
       </c>
       <c r="F10">
-        <v>2.7386940769034721E-5</v>
+        <v>5.9722024442858304E-7</v>
       </c>
       <c r="G10" t="s">
         <v>169</v>
       </c>
-      <c r="H10">
-        <v>3.4756254261292501E-4</v>
-      </c>
-      <c r="I10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>13.516658778480361</v>
+        <v>26.11849747682874</v>
       </c>
       <c r="E11">
-        <v>4.5500508747663933E-2</v>
+        <v>2.9699731885559209E-2</v>
       </c>
       <c r="F11">
-        <v>1.902233621935054E-5</v>
+        <v>2.9766480877012392E-6</v>
       </c>
       <c r="G11" t="s">
         <v>169</v>
       </c>
-      <c r="H11">
-        <v>9.3933737511581099E-5</v>
-      </c>
-      <c r="I11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>13.791109929155111</v>
+        <v>17.847704985311371</v>
       </c>
       <c r="E12">
-        <v>3.5189434441267937E-2</v>
+        <v>1.8632905978004589E-2</v>
       </c>
       <c r="F12">
-        <v>6.6418663808571629E-6</v>
+        <v>4.8773719302883251E-7</v>
       </c>
       <c r="G12" t="s">
         <v>169</v>
       </c>
-      <c r="H12">
-        <v>7.6074854618720847E-5</v>
-      </c>
-      <c r="I12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>9.300661521015904</v>
+        <v>16.223351676640501</v>
       </c>
       <c r="E13">
-        <v>8.0238533275616489E-2</v>
+        <v>5.022025561537951E-2</v>
       </c>
       <c r="F13">
-        <v>2.099118576995485E-4</v>
+        <v>2.7386940769034721E-5</v>
       </c>
       <c r="G13" t="s">
         <v>169</v>
       </c>
-      <c r="H13">
-        <v>4.6119339856969793E-5</v>
-      </c>
-      <c r="I13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14">
-        <v>17.395794507344561</v>
+        <v>13.516658778480361</v>
       </c>
       <c r="E14">
-        <v>6.3754738385994894E-2</v>
+        <v>4.5500508747663933E-2</v>
       </c>
       <c r="F14">
-        <v>6.8641977922538611E-5</v>
+        <v>1.902233621935054E-5</v>
       </c>
       <c r="G14" t="s">
         <v>169</v>
       </c>
-      <c r="H14">
-        <v>1.040501156289542E-3</v>
-      </c>
-      <c r="I14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D15">
-        <v>11.49021058067231</v>
+        <v>13.791109929155111</v>
       </c>
       <c r="E15">
-        <v>8.5764967379633794E-2</v>
+        <v>3.5189434441267937E-2</v>
       </c>
       <c r="F15">
-        <v>2.1941995476272471E-4</v>
+        <v>6.6418663808571629E-6</v>
       </c>
       <c r="G15" t="s">
         <v>169</v>
       </c>
-      <c r="H15">
-        <v>1.2515607323653719E-4</v>
-      </c>
-      <c r="I15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D16">
-        <v>10.158860393984179</v>
+        <v>9.300661521015904</v>
       </c>
       <c r="E16">
-        <v>1.8006171781426161E-2</v>
+        <v>8.0238533275616489E-2</v>
       </c>
       <c r="F16">
-        <v>5.3181031841923174E-7</v>
+        <v>2.099118576995485E-4</v>
       </c>
       <c r="G16" t="s">
         <v>169</v>
       </c>
-      <c r="H16">
-        <v>1.8815181425963959E-5</v>
-      </c>
-      <c r="I16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D17">
-        <v>11.06552503208772</v>
+        <v>17.395794507344561</v>
       </c>
       <c r="E17">
-        <v>3.5078747390956337E-2</v>
+        <v>6.3754738385994894E-2</v>
       </c>
       <c r="F17">
-        <v>6.7579731169204451E-6</v>
+        <v>6.8641977922538611E-5</v>
       </c>
       <c r="G17" t="s">
         <v>169</v>
       </c>
-      <c r="H17">
-        <v>3.0804478380058973E-5</v>
-      </c>
-      <c r="I17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D18">
-        <v>14.480103406126471</v>
+        <v>11.49021058067231</v>
       </c>
       <c r="E18">
-        <v>6.6499791144196997E-3</v>
+        <v>8.5764967379633794E-2</v>
       </c>
       <c r="F18">
-        <v>1.1248655802517469E-8</v>
+        <v>2.1941995476272471E-4</v>
       </c>
       <c r="G18" t="s">
         <v>169</v>
       </c>
-      <c r="H18">
-        <v>5.4245492724434922E-5</v>
-      </c>
-      <c r="I18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D19">
-        <v>9.6397785199583037</v>
+        <v>10.158860393984179</v>
       </c>
       <c r="E19">
-        <v>4.0794879853018197E-2</v>
+        <v>1.8006171781426161E-2</v>
       </c>
       <c r="F19">
-        <v>1.3414837216318149E-5</v>
+        <v>5.3181031841923174E-7</v>
       </c>
       <c r="G19" t="s">
         <v>169</v>
       </c>
-      <c r="H19">
-        <v>2.2532041071350609E-5</v>
-      </c>
-      <c r="I19" t="s">
-        <v>171</v>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>11.06552503208772</v>
+      </c>
+      <c r="E20">
+        <v>3.5078747390956337E-2</v>
+      </c>
+      <c r="F20">
+        <v>6.7579731169204451E-6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21">
+        <v>14.480103406126471</v>
+      </c>
+      <c r="E21">
+        <v>6.6499791144196997E-3</v>
+      </c>
+      <c r="F21">
+        <v>1.1248655802517469E-8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22">
+        <v>9.6397785199583037</v>
+      </c>
+      <c r="E22">
+        <v>4.0794879853018197E-2</v>
+      </c>
+      <c r="F22">
+        <v>1.3414837216318149E-5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>